<commit_message>
调整getQuestion getPaper getSub getActivity四个接口 删除getQuestionByPage getPaperByPage getSubByPage getActivityByPage四个接口 详见接口文档
</commit_message>
<xml_diff>
--- a/doc/服务接口设计文档0522.xlsx
+++ b/doc/服务接口设计文档0522.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17927"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="1000" firstSheet="1" activeTab="9"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" tabRatio="1000" firstSheet="10" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="上传用户头像#" sheetId="33" r:id="rId1"/>
@@ -12,27 +12,23 @@
     <sheet name="用户登陆#" sheetId="4" r:id="rId3"/>
     <sheet name="获取用户资料#" sheetId="31" r:id="rId4"/>
     <sheet name="更新用户资料#" sheetId="32" r:id="rId5"/>
-    <sheet name="获取活动列表#" sheetId="6" r:id="rId6"/>
-    <sheet name="获取活动列表（分页）" sheetId="27" r:id="rId7"/>
-    <sheet name="获取学科列表#" sheetId="5" r:id="rId8"/>
-    <sheet name="获取学科列表（分页）" sheetId="28" r:id="rId9"/>
-    <sheet name="新增、删除用户收藏学科#" sheetId="7" r:id="rId10"/>
-    <sheet name="获取试卷列表#" sheetId="9" r:id="rId11"/>
-    <sheet name="获取试卷列表（分页）" sheetId="29" r:id="rId12"/>
-    <sheet name="获取题目列表#" sheetId="10" r:id="rId13"/>
-    <sheet name="获取题目列表（分页）" sheetId="30" r:id="rId14"/>
-    <sheet name="获取题目详情#" sheetId="11" r:id="rId15"/>
-    <sheet name="提交题目" sheetId="12" r:id="rId16"/>
-    <sheet name="保存答卷进度#" sheetId="13" r:id="rId17"/>
-    <sheet name="获取答卷进度#" sheetId="14" r:id="rId18"/>
-    <sheet name="提交试卷#" sheetId="22" r:id="rId19"/>
-    <sheet name="获取答卷记录#" sheetId="21" r:id="rId20"/>
-    <sheet name="收藏题目#" sheetId="15" r:id="rId21"/>
-    <sheet name="取消收藏#" sheetId="16" r:id="rId22"/>
-    <sheet name="获取收藏夹#" sheetId="20" r:id="rId23"/>
-    <sheet name="加入错题集#" sheetId="24" r:id="rId24"/>
-    <sheet name="移出错题集#" sheetId="26" r:id="rId25"/>
-    <sheet name="获取错题集#" sheetId="25" r:id="rId26"/>
+    <sheet name="获取活动列表（分页）#" sheetId="6" r:id="rId6"/>
+    <sheet name="获取学科列表（分页）#" sheetId="5" r:id="rId7"/>
+    <sheet name="新增、删除用户收藏学科#" sheetId="7" r:id="rId8"/>
+    <sheet name="获取试卷列表（分页）#" sheetId="9" r:id="rId9"/>
+    <sheet name="获取题目列表（分页）#" sheetId="10" r:id="rId10"/>
+    <sheet name="获取题目详情#" sheetId="11" r:id="rId11"/>
+    <sheet name="提交题目" sheetId="12" r:id="rId12"/>
+    <sheet name="保存答卷进度#" sheetId="13" r:id="rId13"/>
+    <sheet name="获取答卷进度#" sheetId="14" r:id="rId14"/>
+    <sheet name="提交试卷#" sheetId="22" r:id="rId15"/>
+    <sheet name="获取答卷记录#" sheetId="21" r:id="rId16"/>
+    <sheet name="收藏题目#" sheetId="15" r:id="rId17"/>
+    <sheet name="取消收藏#" sheetId="16" r:id="rId18"/>
+    <sheet name="获取收藏夹#" sheetId="20" r:id="rId19"/>
+    <sheet name="加入错题集#" sheetId="24" r:id="rId20"/>
+    <sheet name="移出错题集#" sheetId="26" r:id="rId21"/>
+    <sheet name="获取错题集#" sheetId="25" r:id="rId22"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -44,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="579" uniqueCount="207">
   <si>
     <t>Request</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -191,10 +187,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Sub</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>学科对象的数组</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -203,11 +195,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>非必填
-暂时用不到</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Uid</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -228,10 +215,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Paper</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>试卷对象的数组</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -245,10 +228,6 @@
   </si>
   <si>
     <t>试卷ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Ques</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -387,10 +366,6 @@
   </si>
   <si>
     <t>获取答卷记录</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>学科对象的数组</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -460,10 +435,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Response</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>必填：不限制Aid 则为0，不限制Sid则为0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -477,10 +448,6 @@
   </si>
   <si>
     <t>接口：/service/paper/getPaper.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>接口：/service/question/getQuestion.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -705,18 +672,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ID  分区ID
-Aname 分区名称
-Description 描述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ID  学科ID
-Sname 学科名称
-Description 描述</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Paper.ID 试卷ID
 Paper.Name 试卷名称
 Description 描述
@@ -724,10 +679,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Q.ID 题目ID</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Sname 和 Description 都需要urldeCode</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -751,18 +702,6 @@
   <si>
     <t>1:邮箱
 2：手机</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>获取活动列表（ 分页)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>接口：/service/activity/getActivityByPage.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>INT</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -784,23 +723,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>接口：/service/sub/getSubByPage.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>SubList</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>接口：/service/paper/getPaperByPage.php</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PaperList</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>接口：/service/question/getQuestionByPage.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -978,6 +905,10 @@
     <t>100 操作成功
 101 没有这个学科ID、没有这个Uid、之前已经收藏过了
 200 其他错误</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>接口：/service/question/getQuestion.php</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1181,11 +1112,11 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
@@ -1548,7 +1479,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -1556,7 +1487,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -1586,7 +1517,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>18</v>
@@ -1596,12 +1527,12 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>202</v>
-      </c>
-      <c r="C6" s="20"/>
+        <v>186</v>
+      </c>
+      <c r="C6" s="19"/>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1628,13 +1559,13 @@
     </row>
     <row r="9" spans="1:4" ht="77.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="D9" s="3"/>
     </row>
@@ -1653,432 +1584,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="14.75" customWidth="1"/>
-    <col min="3" max="3" width="36.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
-        <v>209</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
-        <v>218</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="6" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>219</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>212</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>213</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>215</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>216</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>214</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="57" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>221</v>
-      </c>
-      <c r="D10" s="1"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A8:D8"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="14.25" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="23.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
-        <v>107</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="27"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
-        <v>103</v>
-      </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="D9" s="18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A7:D7"/>
-    <mergeCell ref="D5:D6"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="14.25" customWidth="1"/>
-    <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="33.25" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
-        <v>179</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="D5" s="26" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="85.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="27"/>
-      <c r="F6" s="9"/>
-    </row>
-    <row r="7" spans="1:6" ht="57" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D7" s="6"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>180</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>46</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>162</v>
-      </c>
-      <c r="D11" s="18" t="s">
-        <v>167</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="A8:D8"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2089,17 +1598,17 @@
     <col min="4" max="4" width="25.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>108</v>
+        <v>206</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -2129,333 +1638,181 @@
     </row>
     <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="8" t="s">
         <v>41</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>43</v>
-      </c>
       <c r="D5" s="31" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C6" s="8" t="s">
         <v>35</v>
       </c>
       <c r="D6" s="32"/>
     </row>
-    <row r="7" spans="1:8" ht="103.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" ht="66.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>34</v>
+        <v>18</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D7" s="33"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+    <row r="8" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" s="30" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="H9" s="13"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C10" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="D10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="H9" s="13"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B10" s="3" t="s">
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:8" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="8" t="s">
+      <c r="C11" s="3" t="s">
         <v>163</v>
       </c>
-      <c r="D11" s="8"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" s="35" t="s">
+        <v>166</v>
+      </c>
+      <c r="B12" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="D12" s="5"/>
+    </row>
+    <row r="13" spans="1:8" ht="57" x14ac:dyDescent="0.2">
+      <c r="A13" s="35"/>
+      <c r="B13" s="35"/>
+      <c r="C13" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D13" s="8" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" s="35"/>
+      <c r="B14" s="35"/>
+      <c r="C14" s="5" t="s">
+        <v>148</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" s="35"/>
+      <c r="B15" s="35"/>
+      <c r="C15" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" s="35"/>
+      <c r="B16" s="35"/>
+      <c r="C16" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="D16" s="34" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="35"/>
+      <c r="B17" s="35"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="34"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="35"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="34"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19" s="35"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>139</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="9">
+    <mergeCell ref="A9:D9"/>
+    <mergeCell ref="A12:A19"/>
+    <mergeCell ref="B12:B19"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="D16:D18"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="D5:D7"/>
-    <mergeCell ref="A8:D8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H19"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="15.625" style="9" customWidth="1"/>
-    <col min="2" max="2" width="12.75" style="9" customWidth="1"/>
-    <col min="3" max="3" width="13" style="9" customWidth="1"/>
-    <col min="4" max="4" width="44.625" style="9" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>181</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="B5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="D5" s="31" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="32"/>
-    </row>
-    <row r="7" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="D7" s="33"/>
-    </row>
-    <row r="8" spans="1:8" ht="71.25" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C8" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D8" s="6"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A9" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B9" s="30"/>
-      <c r="C9" s="30"/>
-      <c r="D9" s="30"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A10" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C10" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="13"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:8" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="35" t="s">
-        <v>182</v>
-      </c>
-      <c r="B12" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" s="5" t="s">
-        <v>159</v>
-      </c>
-      <c r="D12" s="5"/>
-    </row>
-    <row r="13" spans="1:8" ht="57" x14ac:dyDescent="0.2">
-      <c r="A13" s="35"/>
-      <c r="B13" s="35"/>
-      <c r="C13" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="35"/>
-      <c r="B14" s="35"/>
-      <c r="C14" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="D14" s="8" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" s="35"/>
-      <c r="B15" s="35"/>
-      <c r="C15" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A16" s="35"/>
-      <c r="B16" s="35"/>
-      <c r="C16" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="D16" s="34" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17" s="35"/>
-      <c r="B17" s="35"/>
-      <c r="C17" s="36"/>
-      <c r="D17" s="34"/>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="35"/>
-      <c r="B18" s="35"/>
-      <c r="C18" s="36"/>
-      <c r="D18" s="34"/>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A19" s="35"/>
-      <c r="B19" s="35"/>
-      <c r="C19" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>146</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="A12:A19"/>
-    <mergeCell ref="B12:B19"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="A9:D9"/>
-    <mergeCell ref="C16:C18"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D15"/>
   <sheetViews>
@@ -2470,7 +1827,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -2478,7 +1835,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -2508,10 +1865,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
@@ -2542,7 +1899,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B8" s="5" t="s">
         <v>34</v>
@@ -2552,58 +1909,58 @@
     </row>
     <row r="9" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>144</v>
+        <v>137</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="5" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>156</v>
+        <v>149</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>157</v>
+        <v>150</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>158</v>
+        <v>151</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="10" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="36" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B12" s="36" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C12" s="37" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="D12" s="36" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12" customHeight="1" x14ac:dyDescent="0.2">
@@ -2620,16 +1977,16 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>146</v>
+        <v>139</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2649,7 +2006,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -2666,7 +2023,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -2704,12 +2061,12 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
@@ -2720,31 +2077,31 @@
         <v>34</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D8" s="6"/>
     </row>
@@ -2772,13 +2129,13 @@
     </row>
     <row r="11" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>149</v>
+        <v>142</v>
       </c>
       <c r="D11" s="8"/>
     </row>
@@ -2794,7 +2151,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -2811,7 +2168,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -2819,7 +2176,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -2849,17 +2206,17 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>34</v>
@@ -2871,27 +2228,27 @@
     </row>
     <row r="7" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D8" s="6"/>
     </row>
@@ -2919,13 +2276,13 @@
     </row>
     <row r="11" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>150</v>
+        <v>143</v>
       </c>
       <c r="D11" s="8"/>
     </row>
@@ -2941,7 +2298,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D12"/>
   <sheetViews>
@@ -2957,7 +2314,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -2965,7 +2322,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -2995,17 +2352,17 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>34</v>
@@ -3039,52 +2396,52 @@
     </row>
     <row r="9" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="D9" s="6"/>
     </row>
     <row r="10" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>34</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D11" s="6"/>
     </row>
     <row r="12" spans="1:4" ht="40.5" x14ac:dyDescent="0.2">
       <c r="A12" s="12" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B12" s="12" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C12" s="12"/>
       <c r="D12" s="12" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -3100,7 +2457,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -3116,7 +2473,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -3124,7 +2481,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -3154,7 +2511,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -3164,7 +2521,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>18</v>
@@ -3176,49 +2533,49 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="14" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="C7" s="14"/>
       <c r="D7" s="14" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="27" x14ac:dyDescent="0.2">
       <c r="A8" s="14" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B8" s="14" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C8" s="14"/>
       <c r="D8" s="14" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="27" x14ac:dyDescent="0.2">
-      <c r="A9" s="21" t="s">
-        <v>206</v>
-      </c>
-      <c r="B9" s="21" t="s">
-        <v>207</v>
-      </c>
-      <c r="C9" s="21"/>
-      <c r="D9" s="21" t="s">
-        <v>208</v>
+      <c r="A9" s="20" t="s">
+        <v>190</v>
+      </c>
+      <c r="B9" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="C9" s="20"/>
+      <c r="D9" s="20" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="D10" s="6"/>
     </row>
@@ -3246,13 +2603,13 @@
     </row>
     <row r="13" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B13" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>151</v>
+        <v>144</v>
       </c>
       <c r="D13" s="8"/>
     </row>
@@ -3266,6 +2623,532 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="10.625" customWidth="1"/>
+    <col min="3" max="3" width="18.625" customWidth="1"/>
+    <col min="4" max="4" width="19.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
+        <v>82</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="41"/>
+      <c r="B9" s="41"/>
+      <c r="C9" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="41"/>
+      <c r="B10" s="41"/>
+      <c r="C10" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="41"/>
+      <c r="B11" s="41"/>
+      <c r="C11" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="41"/>
+      <c r="B12" s="41"/>
+      <c r="C12" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="42"/>
+      <c r="B13" s="42"/>
+      <c r="C13" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B8:B13"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A6:D6"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="14.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A10" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="D10" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A8:D8"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="15.625" customWidth="1"/>
+    <col min="4" max="4" width="14.375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A9" s="5" t="s">
+        <v>64</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>65</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D9" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A7:D7"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.625" customWidth="1"/>
+    <col min="4" max="4" width="13.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="30"/>
+      <c r="C3" s="30"/>
+      <c r="D3" s="30"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="30" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>158</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A6:D6"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -3293,7 +3176,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -3329,7 +3212,7 @@
         <v>26</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>169</v>
+        <v>159</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>27</v>
@@ -3407,13 +3290,13 @@
         <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>147</v>
+        <v>140</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>19</v>
@@ -3440,532 +3323,6 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="10.625" customWidth="1"/>
-    <col min="3" max="3" width="18.625" customWidth="1"/>
-    <col min="4" max="4" width="19.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
-        <v>86</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>143</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="40" t="s">
-        <v>135</v>
-      </c>
-      <c r="B8" s="40" t="s">
-        <v>136</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="41"/>
-      <c r="B9" s="41"/>
-      <c r="C9" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="41"/>
-      <c r="B10" s="41"/>
-      <c r="C10" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="D10" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A11" s="41"/>
-      <c r="B11" s="41"/>
-      <c r="C11" s="14" t="s">
-        <v>137</v>
-      </c>
-      <c r="D11" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="41"/>
-      <c r="B12" s="41"/>
-      <c r="C12" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" s="14" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="42"/>
-      <c r="B13" s="42"/>
-      <c r="C13" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>138</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B8:B13"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A6:D6"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="14.75" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>122</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B7" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B8" s="30"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C9" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A10" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>152</v>
-      </c>
-      <c r="D10" s="8"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A8:D8"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="15.625" customWidth="1"/>
-    <col min="4" max="4" width="14.375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
-        <v>84</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>125</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="6"/>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
-        <v>80</v>
-      </c>
-      <c r="B6" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="30"/>
-      <c r="C7" s="30"/>
-      <c r="D7" s="30"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A9" s="5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>153</v>
-      </c>
-      <c r="D9" s="8"/>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A7:D7"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="11.625" customWidth="1"/>
-    <col min="4" max="4" width="13.875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
-        <v>127</v>
-      </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="29" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="30"/>
-      <c r="C3" s="30"/>
-      <c r="D3" s="30"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="30" t="s">
-        <v>1</v>
-      </c>
-      <c r="B6" s="30"/>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="5" t="s">
-        <v>124</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>166</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A6:D6"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -3979,7 +3336,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -3987,7 +3344,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -4017,7 +3374,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -4027,7 +3384,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>18</v>
@@ -4061,13 +3418,13 @@
     </row>
     <row r="9" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>154</v>
+        <v>147</v>
       </c>
       <c r="D9" s="8"/>
     </row>
@@ -4083,7 +3440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -4099,7 +3456,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -4107,7 +3464,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -4137,7 +3494,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -4147,7 +3504,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>18</v>
@@ -4181,13 +3538,13 @@
     </row>
     <row r="9" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B9" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D9" s="8"/>
     </row>
@@ -4203,7 +3560,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D8"/>
   <sheetViews>
@@ -4219,7 +3576,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="28" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="B1" s="28"/>
       <c r="C1" s="28"/>
@@ -4227,7 +3584,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="29" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
@@ -4257,7 +3614,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="11" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B5" s="11"/>
       <c r="C5" s="11"/>
@@ -4289,13 +3646,13 @@
     </row>
     <row r="8" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D8" s="8"/>
     </row>
@@ -4336,7 +3693,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -4450,13 +3807,13 @@
         <v>18</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>148</v>
+        <v>141</v>
       </c>
       <c r="D11" s="1"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>159</v>
+        <v>152</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>19</v>
@@ -4498,7 +3855,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -4506,7 +3863,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -4536,7 +3893,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>18</v>
@@ -4568,7 +3925,7 @@
     </row>
     <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -4576,7 +3933,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -4584,7 +3941,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="B10" s="3"/>
       <c r="C10" s="3"/>
@@ -4592,17 +3949,17 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="C11" s="3"/>
       <c r="D11" s="3"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -4610,10 +3967,10 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
@@ -4666,7 +4023,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -4674,7 +4031,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -4704,7 +4061,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>18</v>
@@ -4714,17 +4071,17 @@
     </row>
     <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="B6" s="3"/>
       <c r="C6" s="25" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="D6" s="3"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="B7" s="3"/>
       <c r="C7" s="25"/>
@@ -4732,7 +4089,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="25"/>
@@ -4740,7 +4097,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="B9" s="3"/>
       <c r="C9" s="25"/>
@@ -4773,10 +4130,10 @@
         <v>20</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="D12" s="3"/>
     </row>
@@ -4796,10 +4153,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4811,7 +4168,7 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -4819,7 +4176,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -4847,10 +4204,16 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
+    <row r="5" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>160</v>
+      </c>
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -4875,18 +4238,30 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" s="8" t="s">
-        <v>160</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>165</v>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D8" s="3"/>
+    </row>
+    <row r="9" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>189</v>
+      </c>
+      <c r="D9" s="17" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -4903,22 +4278,22 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="19.75" customWidth="1"/>
-    <col min="3" max="3" width="27.5" customWidth="1"/>
-    <col min="4" max="4" width="31.625" customWidth="1"/>
+    <col min="2" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="20.25" customWidth="1"/>
+    <col min="4" max="4" width="33.125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>170</v>
+        <v>33</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -4926,13 +4301,13 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>171</v>
+        <v>201</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
       <c r="D2" s="23"/>
     </row>
-    <row r="3" spans="1:4" ht="28.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>0</v>
       </c>
@@ -4954,64 +4329,90 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>174</v>
+        <v>37</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D5" s="6"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="D5" s="6" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="24" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B9" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B8" s="3" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" ht="57" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>205</v>
-      </c>
-      <c r="D9" s="17" t="s">
-        <v>165</v>
+      <c r="C10" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>188</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -5019,7 +4420,7 @@
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A2:D2"/>
     <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A8:D8"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5032,19 +4433,18 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:D7"/>
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="20.25" customWidth="1"/>
-    <col min="4" max="4" width="33.125" customWidth="1"/>
+    <col min="2" max="2" width="14.75" customWidth="1"/>
+    <col min="3" max="3" width="36.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="22" t="s">
-        <v>33</v>
+        <v>193</v>
       </c>
       <c r="B1" s="22"/>
       <c r="C1" s="22"/>
@@ -5052,7 +4452,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="23" t="s">
-        <v>177</v>
+        <v>202</v>
       </c>
       <c r="B2" s="23"/>
       <c r="C2" s="23"/>
@@ -5080,7 +4480,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>38</v>
       </c>
@@ -5089,174 +4489,36 @@
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>41</v>
+        <v>203</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>196</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A7" s="24" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="8" t="s">
-        <v>161</v>
-      </c>
-      <c r="D10" s="16" t="s">
-        <v>164</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:D2"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A7:D7"/>
-  </mergeCells>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="20.25" customWidth="1"/>
-    <col min="4" max="4" width="33.125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" s="23" t="s">
-        <v>217</v>
-      </c>
-      <c r="B2" s="23"/>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3" s="24"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="6" t="s">
-        <v>220</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D6" s="8" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" ht="57" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>174</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>172</v>
-      </c>
-      <c r="C7" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D7" s="6"/>
+        <v>197</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>200</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A8" s="24" t="s">
@@ -5280,31 +4542,17 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A10" s="3" t="s">
-        <v>175</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" ht="57" x14ac:dyDescent="0.2">
-      <c r="A11" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>204</v>
-      </c>
-      <c r="D11" s="16" t="s">
-        <v>164</v>
-      </c>
+    <row r="10" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>182</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D10" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -5315,6 +4563,159 @@
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.25" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="23" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="42.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="27"/>
+      <c r="F6" s="9"/>
+    </row>
+    <row r="7" spans="1:6" ht="57" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="24"/>
+      <c r="C8" s="24"/>
+      <c r="D8" s="24"/>
+    </row>
+    <row r="9" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" ht="71.25" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A8:D8"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:D2"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="D5:D6"/>
+  </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>